<commit_message>
Consolidate files with Windows version. Include new documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Connections.xlsx
+++ b/Documentation/Connections.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FMC" sheetId="1" r:id="rId1"/>
-    <sheet name="I2C" sheetId="2" r:id="rId2"/>
-    <sheet name="HDMI" sheetId="3" r:id="rId3"/>
-    <sheet name="Added SFP" sheetId="4" r:id="rId4"/>
-    <sheet name="LEDs" sheetId="5" r:id="rId5"/>
+    <sheet name="FMC_V1E" sheetId="6" r:id="rId2"/>
+    <sheet name="I2C" sheetId="2" r:id="rId3"/>
+    <sheet name="HDMI" sheetId="3" r:id="rId4"/>
+    <sheet name="Added SFP" sheetId="4" r:id="rId5"/>
+    <sheet name="LEDs" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="515">
   <si>
     <t>BEAM_TRIGGER_P&lt;0&gt;</t>
   </si>
@@ -1655,13 +1656,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1968,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,11 +1985,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="2" t="s">
         <v>40</v>
       </c>
@@ -5881,6 +5882,3922 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I302"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H14" si="0">"set_property PACKAGE_PIN " &amp;E3 &amp; " [get_ports {" &amp; F3 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN B1 [get_ports {threshold_discr_p_i[0]}]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN C4 [get_ports {threshold_discr_p_i[1]}]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN K2 [get_ports {threshold_discr_p_i[2]}]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN C6 [get_ports {threshold_discr_p_i[3]}]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN J4 [get_ports {threshold_discr_p_i[4]}]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN H1 [get_ports {threshold_discr_p_i[5]}]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN A1 [get_ports {threshold_discr_n_i[0]}]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN B4 [get_ports {threshold_discr_n_i[1]}]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN K1 [get_ports {threshold_discr_n_i[2]}]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN C5 [get_ports {threshold_discr_n_i[3]}]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN H4 [get_ports {threshold_discr_n_i[4]}]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>set_property PACKAGE_PIN G1 [get_ports {threshold_discr_n_i[5]}]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" ref="H17:H20" si="1">"set_property PACKAGE_PIN " &amp;E17 &amp; " [get_ports {" &amp; F17 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN T5 [get_ports {sysclk_40_i_p}]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>set_property PACKAGE_PIN T4 [get_ports {sysclk_40_i_n}]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>set_property PACKAGE_PIN E3 [get_ports {sysclk_50_o_p}]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>set_property PACKAGE_PIN D3 [get_ports {sysclk_50_o_n}]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" ref="H22:H24" si="2">"set_property PACKAGE_PIN " &amp;E22 &amp; " [get_ports {" &amp; F22 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN C2 [get_ports {i2c_reset}]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>set_property PACKAGE_PIN F6 [get_ports {gpio}]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>set_property PACKAGE_PIN C1 [get_ports {clk_gen_rst}]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" ref="H37:H50" si="3">"set_property PACKAGE_PIN " &amp;E37 &amp; " [get_ports {" &amp; F37 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN P5 [get_ports {cont_i[0]}]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN P3 [get_ports {cont_i[1]}]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN N6 [get_ports {cont_i[2]}]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN L5 [get_ports {cont_i[3]}]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN M1 [get_ports {spare_i[0]}]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN N4 [get_ports {spare_i[1]}]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN N1 [get_ports {spare_i[2]}]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN M2 [get_ports {spare_i[3]}]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN R5 [get_ports {triggers_i[0]}]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN R2 [get_ports {triggers_i[1]}]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN T1 [get_ports {triggers_i[2]}]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="3"/>
+        <v>set_property PACKAGE_PIN V1 [get_ports {triggers_i[3]}]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" ref="H52:H60" si="4">"set_property PACKAGE_PIN " &amp;E52 &amp; " [get_ports {" &amp; F52 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN T6 [get_ports {busy_i[0]}]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN U3 [get_ports {busy_i[1]}]</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN T8 [get_ports {busy_i[2]}]</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN L4 [get_ports {busy_i[3]}]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN L3 [get_ports {dut_clk_i[0]}]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN F3 [get_ports {dut_clk_i[1]}]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN D2 [get_ports {dut_clk_i[2]}]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="4"/>
+        <v>set_property PACKAGE_PIN G3 [get_ports {dut_clk_i[3]}]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" ref="H62:H75" si="5">"set_property PACKAGE_PIN " &amp;E62 &amp; " [get_ports {" &amp; F62 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN N5 [get_ports {cont_o[0]}]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN P4 [get_ports {cont_o[1]}]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN M6 [get_ports {cont_o[2]}]</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN L6 [get_ports {cont_o[3]}]</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN L1 [get_ports {spare_o[0]}]</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN M4 [get_ports {spare_o[1]}]</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN N2 [get_ports {spare_o[2]}]</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN M3 [get_ports {spare_o[3]}]</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN R6 [get_ports {triggers_o[0]}]</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN P2 [get_ports {triggers_o[1]}]</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN R1 [get_ports {triggers_o[2]}]</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="5"/>
+        <v>set_property PACKAGE_PIN U1 [get_ports {triggers_o[3]}]</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H77" t="str">
+        <f>"set_property PACKAGE_PIN " &amp;E77 &amp; " [get_ports {" &amp; F77 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN R7 [get_ports {busy_o[0]}]</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" ref="H78:H85" si="6">"set_property PACKAGE_PIN " &amp;E78 &amp; " [get_ports {" &amp; F78 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN U4 [get_ports {busy_o[1]}]</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H79" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN R8 [get_ports {busy_o[2]}]</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN K5 [get_ports {busy_o[3]}]</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H82" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN K3 [get_ports {dut_clk_o[0]}]</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H83" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN F4 [get_ports {dut_clk_o[1]}]</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H84" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN E2 [get_ports {dut_clk_o[2]}]</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H85" t="str">
+        <f t="shared" si="6"/>
+        <v>set_property PACKAGE_PIN G4 [get_ports {dut_clk_o[3]}]</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="5"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="5"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="5"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="5"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="5"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="5"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="5"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="5"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="5"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="5"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="5"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="5"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="5"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="5"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="5"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="5"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="5"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="5"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="5"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="5"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="5"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="5"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="5"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="5"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="5"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="5"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="5"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="5"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="5"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="5"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="5"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="5"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="5"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="5"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="5"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="5"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="5"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="5"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="5"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="5"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="5"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="5"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="5"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="5"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="5"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="5"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="5"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="5"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="5"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="5"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="5"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="5"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="5"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="5"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="5"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="5"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="5"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="5"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="5"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="5"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="5"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="5"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="5"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="5"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="5"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="5"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="5"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="5"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="5"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="5"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="5"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="5"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="5"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="5"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="5"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="5"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="5"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="5"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="5"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="5"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="5"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="5"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="5"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="5"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="5"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="5"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="4"/>
+      <c r="B182" s="4"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="5"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="4"/>
+      <c r="B183" s="4"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="5"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="4"/>
+      <c r="B184" s="4"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="5"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="4"/>
+      <c r="B185" s="4"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="5"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="4"/>
+      <c r="B186" s="4"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="5"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="4"/>
+      <c r="B187" s="4"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="5"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="4"/>
+      <c r="B188" s="4"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="5"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="4"/>
+      <c r="B189" s="4"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="5"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="4"/>
+      <c r="B190" s="4"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="5"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="4"/>
+      <c r="B191" s="4"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="5"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="4"/>
+      <c r="B192" s="4"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="5"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="4"/>
+      <c r="B193" s="4"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="5"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="4"/>
+      <c r="B194" s="4"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="5"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="4"/>
+      <c r="B195" s="4"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="4"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="5"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" s="4"/>
+      <c r="B196" s="4"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="4"/>
+      <c r="F196" s="4"/>
+      <c r="G196" s="5"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" s="4"/>
+      <c r="B197" s="4"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="4"/>
+      <c r="F197" s="4"/>
+      <c r="G197" s="5"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="4"/>
+      <c r="B198" s="4"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="4"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="5"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="4"/>
+      <c r="B199" s="4"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="4"/>
+      <c r="F199" s="4"/>
+      <c r="G199" s="5"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" s="4"/>
+      <c r="B200" s="4"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="4"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="5"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" s="4"/>
+      <c r="B201" s="4"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="4"/>
+      <c r="F201" s="4"/>
+      <c r="G201" s="5"/>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" s="4"/>
+      <c r="B202" s="4"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="4"/>
+      <c r="E202" s="4"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="5"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" s="4"/>
+      <c r="B203" s="4"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="4"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="5"/>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="4"/>
+      <c r="B204" s="4"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="4"/>
+      <c r="E204" s="4"/>
+      <c r="F204" s="4"/>
+      <c r="G204" s="5"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="4"/>
+      <c r="B205" s="4"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="4"/>
+      <c r="F205" s="4"/>
+      <c r="G205" s="5"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" s="4"/>
+      <c r="B206" s="4"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="4"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="5"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" s="4"/>
+      <c r="B207" s="4"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="4"/>
+      <c r="E207" s="4"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="5"/>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" s="4"/>
+      <c r="B208" s="4"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="4"/>
+      <c r="E208" s="4"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="5"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="4"/>
+      <c r="B209" s="4"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="4"/>
+      <c r="E209" s="4"/>
+      <c r="F209" s="4"/>
+      <c r="G209" s="5"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" s="4"/>
+      <c r="B210" s="4"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="4"/>
+      <c r="E210" s="4"/>
+      <c r="F210" s="4"/>
+      <c r="G210" s="5"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="4"/>
+      <c r="B211" s="4"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="4"/>
+      <c r="E211" s="4"/>
+      <c r="F211" s="4"/>
+      <c r="G211" s="5"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="4"/>
+      <c r="B212" s="4"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="4"/>
+      <c r="E212" s="4"/>
+      <c r="F212" s="4"/>
+      <c r="G212" s="5"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" s="4"/>
+      <c r="B213" s="4"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="4"/>
+      <c r="E213" s="4"/>
+      <c r="F213" s="4"/>
+      <c r="G213" s="5"/>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214" s="4"/>
+      <c r="B214" s="4"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="4"/>
+      <c r="E214" s="4"/>
+      <c r="F214" s="4"/>
+      <c r="G214" s="5"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="4"/>
+      <c r="B215" s="4"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="4"/>
+      <c r="F215" s="4"/>
+      <c r="G215" s="5"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="4"/>
+      <c r="B216" s="4"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="4"/>
+      <c r="E216" s="4"/>
+      <c r="F216" s="4"/>
+      <c r="G216" s="5"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217" s="4"/>
+      <c r="B217" s="4"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="4"/>
+      <c r="E217" s="4"/>
+      <c r="F217" s="4"/>
+      <c r="G217" s="5"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218" s="4"/>
+      <c r="B218" s="4"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="4"/>
+      <c r="E218" s="4"/>
+      <c r="F218" s="4"/>
+      <c r="G218" s="5"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="4"/>
+      <c r="B219" s="4"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="4"/>
+      <c r="E219" s="4"/>
+      <c r="F219" s="4"/>
+      <c r="G219" s="5"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="4"/>
+      <c r="B220" s="4"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="4"/>
+      <c r="E220" s="4"/>
+      <c r="F220" s="4"/>
+      <c r="G220" s="5"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221" s="4"/>
+      <c r="B221" s="4"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="4"/>
+      <c r="E221" s="4"/>
+      <c r="F221" s="4"/>
+      <c r="G221" s="5"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222" s="4"/>
+      <c r="B222" s="4"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="4"/>
+      <c r="E222" s="4"/>
+      <c r="F222" s="4"/>
+      <c r="G222" s="5"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223" s="4"/>
+      <c r="B223" s="4"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="4"/>
+      <c r="E223" s="4"/>
+      <c r="F223" s="4"/>
+      <c r="G223" s="5"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224" s="4"/>
+      <c r="B224" s="4"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="4"/>
+      <c r="E224" s="4"/>
+      <c r="F224" s="4"/>
+      <c r="G224" s="5"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225" s="4"/>
+      <c r="B225" s="4"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="4"/>
+      <c r="E225" s="4"/>
+      <c r="F225" s="4"/>
+      <c r="G225" s="5"/>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A226" s="4"/>
+      <c r="B226" s="4"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="4"/>
+      <c r="E226" s="4"/>
+      <c r="F226" s="4"/>
+      <c r="G226" s="5"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A227" s="4"/>
+      <c r="B227" s="4"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="4"/>
+      <c r="E227" s="4"/>
+      <c r="F227" s="4"/>
+      <c r="G227" s="5"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228" s="4"/>
+      <c r="B228" s="4"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="4"/>
+      <c r="E228" s="4"/>
+      <c r="F228" s="4"/>
+      <c r="G228" s="5"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="4"/>
+      <c r="B229" s="4"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="4"/>
+      <c r="E229" s="4"/>
+      <c r="F229" s="4"/>
+      <c r="G229" s="5"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="4"/>
+      <c r="B230" s="4"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="4"/>
+      <c r="E230" s="4"/>
+      <c r="F230" s="4"/>
+      <c r="G230" s="5"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" s="4"/>
+      <c r="B231" s="4"/>
+      <c r="C231" s="5"/>
+      <c r="D231" s="4"/>
+      <c r="E231" s="4"/>
+      <c r="F231" s="4"/>
+      <c r="G231" s="5"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" s="4"/>
+      <c r="B232" s="4"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="4"/>
+      <c r="E232" s="4"/>
+      <c r="F232" s="4"/>
+      <c r="G232" s="5"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="4"/>
+      <c r="B233" s="4"/>
+      <c r="C233" s="5"/>
+      <c r="D233" s="4"/>
+      <c r="E233" s="4"/>
+      <c r="F233" s="4"/>
+      <c r="G233" s="5"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" s="4"/>
+      <c r="B234" s="4"/>
+      <c r="C234" s="5"/>
+      <c r="D234" s="4"/>
+      <c r="E234" s="4"/>
+      <c r="F234" s="4"/>
+      <c r="G234" s="5"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="4"/>
+      <c r="B235" s="4"/>
+      <c r="C235" s="5"/>
+      <c r="D235" s="4"/>
+      <c r="E235" s="4"/>
+      <c r="F235" s="4"/>
+      <c r="G235" s="5"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="4"/>
+      <c r="B236" s="4"/>
+      <c r="C236" s="5"/>
+      <c r="D236" s="4"/>
+      <c r="E236" s="4"/>
+      <c r="F236" s="4"/>
+      <c r="G236" s="5"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="4"/>
+      <c r="B237" s="4"/>
+      <c r="C237" s="5"/>
+      <c r="D237" s="4"/>
+      <c r="E237" s="4"/>
+      <c r="F237" s="4"/>
+      <c r="G237" s="5"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="4"/>
+      <c r="B238" s="4"/>
+      <c r="C238" s="5"/>
+      <c r="D238" s="4"/>
+      <c r="E238" s="4"/>
+      <c r="F238" s="4"/>
+      <c r="G238" s="5"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="4"/>
+      <c r="B239" s="4"/>
+      <c r="C239" s="5"/>
+      <c r="D239" s="4"/>
+      <c r="E239" s="4"/>
+      <c r="F239" s="4"/>
+      <c r="G239" s="5"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="4"/>
+      <c r="B240" s="4"/>
+      <c r="C240" s="5"/>
+      <c r="D240" s="4"/>
+      <c r="E240" s="4"/>
+      <c r="F240" s="4"/>
+      <c r="G240" s="5"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="4"/>
+      <c r="B241" s="4"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="4"/>
+      <c r="E241" s="4"/>
+      <c r="F241" s="4"/>
+      <c r="G241" s="5"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="4"/>
+      <c r="B242" s="4"/>
+      <c r="C242" s="5"/>
+      <c r="D242" s="4"/>
+      <c r="E242" s="4"/>
+      <c r="F242" s="4"/>
+      <c r="G242" s="5"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="4"/>
+      <c r="B243" s="4"/>
+      <c r="C243" s="5"/>
+      <c r="D243" s="4"/>
+      <c r="E243" s="4"/>
+      <c r="F243" s="4"/>
+      <c r="G243" s="5"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="4"/>
+      <c r="B244" s="4"/>
+      <c r="C244" s="5"/>
+      <c r="D244" s="4"/>
+      <c r="E244" s="4"/>
+      <c r="F244" s="4"/>
+      <c r="G244" s="5"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="4"/>
+      <c r="B245" s="4"/>
+      <c r="C245" s="5"/>
+      <c r="D245" s="4"/>
+      <c r="E245" s="4"/>
+      <c r="F245" s="4"/>
+      <c r="G245" s="5"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="4"/>
+      <c r="B246" s="4"/>
+      <c r="C246" s="5"/>
+      <c r="D246" s="4"/>
+      <c r="E246" s="4"/>
+      <c r="F246" s="4"/>
+      <c r="G246" s="5"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="4"/>
+      <c r="B247" s="4"/>
+      <c r="C247" s="5"/>
+      <c r="D247" s="4"/>
+      <c r="E247" s="4"/>
+      <c r="F247" s="4"/>
+      <c r="G247" s="5"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="4"/>
+      <c r="B248" s="4"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="4"/>
+      <c r="E248" s="4"/>
+      <c r="F248" s="4"/>
+      <c r="G248" s="5"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="4"/>
+      <c r="B249" s="4"/>
+      <c r="C249" s="5"/>
+      <c r="D249" s="4"/>
+      <c r="E249" s="4"/>
+      <c r="F249" s="4"/>
+      <c r="G249" s="5"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="4"/>
+      <c r="B250" s="4"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="4"/>
+      <c r="E250" s="4"/>
+      <c r="F250" s="4"/>
+      <c r="G250" s="5"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="4"/>
+      <c r="B251" s="4"/>
+      <c r="C251" s="5"/>
+      <c r="D251" s="4"/>
+      <c r="E251" s="4"/>
+      <c r="F251" s="4"/>
+      <c r="G251" s="5"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="4"/>
+      <c r="B252" s="4"/>
+      <c r="C252" s="5"/>
+      <c r="D252" s="4"/>
+      <c r="E252" s="4"/>
+      <c r="F252" s="4"/>
+      <c r="G252" s="5"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="4"/>
+      <c r="B253" s="4"/>
+      <c r="C253" s="5"/>
+      <c r="D253" s="4"/>
+      <c r="E253" s="4"/>
+      <c r="F253" s="4"/>
+      <c r="G253" s="5"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="4"/>
+      <c r="B254" s="4"/>
+      <c r="C254" s="5"/>
+      <c r="D254" s="4"/>
+      <c r="E254" s="4"/>
+      <c r="F254" s="4"/>
+      <c r="G254" s="5"/>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="4"/>
+      <c r="B255" s="4"/>
+      <c r="C255" s="5"/>
+      <c r="D255" s="4"/>
+      <c r="E255" s="4"/>
+      <c r="F255" s="4"/>
+      <c r="G255" s="5"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="4"/>
+      <c r="B256" s="4"/>
+      <c r="C256" s="5"/>
+      <c r="D256" s="4"/>
+      <c r="E256" s="4"/>
+      <c r="F256" s="4"/>
+      <c r="G256" s="5"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="4"/>
+      <c r="B257" s="4"/>
+      <c r="C257" s="5"/>
+      <c r="D257" s="4"/>
+      <c r="E257" s="4"/>
+      <c r="F257" s="4"/>
+      <c r="G257" s="5"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="4"/>
+      <c r="B258" s="4"/>
+      <c r="C258" s="5"/>
+      <c r="D258" s="4"/>
+      <c r="E258" s="4"/>
+      <c r="F258" s="4"/>
+      <c r="G258" s="5"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="4"/>
+      <c r="B259" s="4"/>
+      <c r="C259" s="5"/>
+      <c r="D259" s="4"/>
+      <c r="E259" s="4"/>
+      <c r="F259" s="4"/>
+      <c r="G259" s="5"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="4"/>
+      <c r="B260" s="4"/>
+      <c r="C260" s="5"/>
+      <c r="D260" s="4"/>
+      <c r="E260" s="4"/>
+      <c r="F260" s="4"/>
+      <c r="G260" s="5"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="4"/>
+      <c r="B261" s="4"/>
+      <c r="C261" s="5"/>
+      <c r="D261" s="4"/>
+      <c r="E261" s="4"/>
+      <c r="F261" s="4"/>
+      <c r="G261" s="5"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="4"/>
+      <c r="B262" s="4"/>
+      <c r="C262" s="5"/>
+      <c r="D262" s="4"/>
+      <c r="E262" s="4"/>
+      <c r="F262" s="4"/>
+      <c r="G262" s="5"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="4"/>
+      <c r="B263" s="4"/>
+      <c r="C263" s="5"/>
+      <c r="D263" s="4"/>
+      <c r="E263" s="4"/>
+      <c r="F263" s="4"/>
+      <c r="G263" s="5"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="4"/>
+      <c r="B264" s="4"/>
+      <c r="C264" s="5"/>
+      <c r="D264" s="4"/>
+      <c r="E264" s="4"/>
+      <c r="F264" s="4"/>
+      <c r="G264" s="5"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="4"/>
+      <c r="B265" s="4"/>
+      <c r="C265" s="5"/>
+      <c r="D265" s="4"/>
+      <c r="E265" s="4"/>
+      <c r="F265" s="4"/>
+      <c r="G265" s="5"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="4"/>
+      <c r="B266" s="4"/>
+      <c r="C266" s="5"/>
+      <c r="D266" s="4"/>
+      <c r="E266" s="4"/>
+      <c r="F266" s="4"/>
+      <c r="G266" s="5"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="4"/>
+      <c r="B267" s="4"/>
+      <c r="C267" s="5"/>
+      <c r="D267" s="4"/>
+      <c r="E267" s="4"/>
+      <c r="F267" s="4"/>
+      <c r="G267" s="5"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="4"/>
+      <c r="B268" s="4"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="4"/>
+      <c r="E268" s="4"/>
+      <c r="F268" s="4"/>
+      <c r="G268" s="5"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="4"/>
+      <c r="B269" s="4"/>
+      <c r="C269" s="5"/>
+      <c r="D269" s="4"/>
+      <c r="E269" s="4"/>
+      <c r="F269" s="4"/>
+      <c r="G269" s="5"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="4"/>
+      <c r="B270" s="4"/>
+      <c r="C270" s="5"/>
+      <c r="D270" s="4"/>
+      <c r="E270" s="4"/>
+      <c r="F270" s="4"/>
+      <c r="G270" s="5"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="4"/>
+      <c r="B271" s="4"/>
+      <c r="C271" s="5"/>
+      <c r="D271" s="4"/>
+      <c r="E271" s="4"/>
+      <c r="F271" s="4"/>
+      <c r="G271" s="5"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="4"/>
+      <c r="B272" s="4"/>
+      <c r="C272" s="5"/>
+      <c r="D272" s="4"/>
+      <c r="E272" s="4"/>
+      <c r="F272" s="4"/>
+      <c r="G272" s="5"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="4"/>
+      <c r="B273" s="4"/>
+      <c r="C273" s="5"/>
+      <c r="D273" s="4"/>
+      <c r="E273" s="4"/>
+      <c r="F273" s="4"/>
+      <c r="G273" s="5"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="4"/>
+      <c r="B274" s="4"/>
+      <c r="C274" s="5"/>
+      <c r="D274" s="4"/>
+      <c r="E274" s="4"/>
+      <c r="F274" s="4"/>
+      <c r="G274" s="5"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="4"/>
+      <c r="B275" s="4"/>
+      <c r="C275" s="5"/>
+      <c r="D275" s="4"/>
+      <c r="E275" s="4"/>
+      <c r="F275" s="4"/>
+      <c r="G275" s="5"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="4"/>
+      <c r="B276" s="4"/>
+      <c r="C276" s="5"/>
+      <c r="D276" s="4"/>
+      <c r="E276" s="4"/>
+      <c r="F276" s="4"/>
+      <c r="G276" s="5"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="4"/>
+      <c r="B277" s="4"/>
+      <c r="C277" s="5"/>
+      <c r="D277" s="4"/>
+      <c r="E277" s="4"/>
+      <c r="F277" s="4"/>
+      <c r="G277" s="5"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="4"/>
+      <c r="B278" s="4"/>
+      <c r="C278" s="5"/>
+      <c r="D278" s="4"/>
+      <c r="E278" s="4"/>
+      <c r="F278" s="4"/>
+      <c r="G278" s="5"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="4"/>
+      <c r="B279" s="4"/>
+      <c r="C279" s="5"/>
+      <c r="D279" s="4"/>
+      <c r="E279" s="4"/>
+      <c r="F279" s="4"/>
+      <c r="G279" s="5"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="4"/>
+      <c r="B280" s="4"/>
+      <c r="C280" s="5"/>
+      <c r="D280" s="4"/>
+      <c r="E280" s="4"/>
+      <c r="F280" s="4"/>
+      <c r="G280" s="5"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="4"/>
+      <c r="B281" s="4"/>
+      <c r="C281" s="5"/>
+      <c r="D281" s="4"/>
+      <c r="E281" s="4"/>
+      <c r="F281" s="4"/>
+      <c r="G281" s="5"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="4"/>
+      <c r="B282" s="4"/>
+      <c r="C282" s="5"/>
+      <c r="D282" s="4"/>
+      <c r="E282" s="4"/>
+      <c r="F282" s="4"/>
+      <c r="G282" s="5"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="4"/>
+      <c r="B283" s="4"/>
+      <c r="C283" s="5"/>
+      <c r="D283" s="4"/>
+      <c r="E283" s="4"/>
+      <c r="F283" s="4"/>
+      <c r="G283" s="5"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="4"/>
+      <c r="B284" s="4"/>
+      <c r="C284" s="5"/>
+      <c r="D284" s="4"/>
+      <c r="E284" s="4"/>
+      <c r="F284" s="4"/>
+      <c r="G284" s="5"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="4"/>
+      <c r="B285" s="4"/>
+      <c r="C285" s="5"/>
+      <c r="D285" s="4"/>
+      <c r="E285" s="4"/>
+      <c r="F285" s="4"/>
+      <c r="G285" s="5"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="4"/>
+      <c r="B286" s="4"/>
+      <c r="C286" s="5"/>
+      <c r="D286" s="4"/>
+      <c r="E286" s="4"/>
+      <c r="F286" s="4"/>
+      <c r="G286" s="5"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="4"/>
+      <c r="B287" s="4"/>
+      <c r="C287" s="5"/>
+      <c r="D287" s="4"/>
+      <c r="E287" s="4"/>
+      <c r="F287" s="4"/>
+      <c r="G287" s="5"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="4"/>
+      <c r="B288" s="4"/>
+      <c r="C288" s="5"/>
+      <c r="D288" s="4"/>
+      <c r="E288" s="4"/>
+      <c r="F288" s="4"/>
+      <c r="G288" s="5"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="4"/>
+      <c r="B289" s="4"/>
+      <c r="C289" s="5"/>
+      <c r="D289" s="4"/>
+      <c r="E289" s="4"/>
+      <c r="F289" s="4"/>
+      <c r="G289" s="5"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="4"/>
+      <c r="B290" s="4"/>
+      <c r="C290" s="5"/>
+      <c r="D290" s="4"/>
+      <c r="E290" s="4"/>
+      <c r="F290" s="4"/>
+      <c r="G290" s="5"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="4"/>
+      <c r="B291" s="4"/>
+      <c r="C291" s="5"/>
+      <c r="D291" s="4"/>
+      <c r="E291" s="4"/>
+      <c r="F291" s="4"/>
+      <c r="G291" s="5"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="4"/>
+      <c r="B292" s="4"/>
+      <c r="C292" s="5"/>
+      <c r="D292" s="4"/>
+      <c r="E292" s="4"/>
+      <c r="F292" s="4"/>
+      <c r="G292" s="5"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="4"/>
+      <c r="B293" s="4"/>
+      <c r="C293" s="5"/>
+      <c r="D293" s="4"/>
+      <c r="E293" s="4"/>
+      <c r="F293" s="4"/>
+      <c r="G293" s="5"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="4"/>
+      <c r="B294" s="4"/>
+      <c r="C294" s="5"/>
+      <c r="D294" s="4"/>
+      <c r="E294" s="4"/>
+      <c r="F294" s="4"/>
+      <c r="G294" s="5"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="4"/>
+      <c r="B295" s="4"/>
+      <c r="C295" s="5"/>
+      <c r="D295" s="4"/>
+      <c r="E295" s="4"/>
+      <c r="F295" s="4"/>
+      <c r="G295" s="5"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="4"/>
+      <c r="B296" s="4"/>
+      <c r="C296" s="5"/>
+      <c r="D296" s="4"/>
+      <c r="E296" s="4"/>
+      <c r="F296" s="4"/>
+      <c r="G296" s="5"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="4"/>
+      <c r="B297" s="4"/>
+      <c r="C297" s="5"/>
+      <c r="D297" s="4"/>
+      <c r="E297" s="4"/>
+      <c r="F297" s="4"/>
+      <c r="G297" s="5"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="4"/>
+      <c r="B298" s="4"/>
+      <c r="C298" s="5"/>
+      <c r="D298" s="4"/>
+      <c r="E298" s="4"/>
+      <c r="F298" s="4"/>
+      <c r="G298" s="5"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="4"/>
+      <c r="B299" s="4"/>
+      <c r="C299" s="5"/>
+      <c r="D299" s="4"/>
+      <c r="E299" s="4"/>
+      <c r="F299" s="4"/>
+      <c r="G299" s="5"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="4"/>
+      <c r="B300" s="4"/>
+      <c r="C300" s="5"/>
+      <c r="D300" s="4"/>
+      <c r="E300" s="4"/>
+      <c r="F300" s="4"/>
+      <c r="G300" s="5"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="4"/>
+      <c r="B301" s="4"/>
+      <c r="C301" s="5"/>
+      <c r="D301" s="4"/>
+      <c r="E301" s="4"/>
+      <c r="F301" s="4"/>
+      <c r="G301" s="5"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C302" s="5"/>
+      <c r="D302" s="4"/>
+      <c r="E302" s="4"/>
+      <c r="F302" s="4"/>
+      <c r="G302" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
@@ -6044,7 +9961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
@@ -6325,7 +10242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D31"/>
   <sheetViews>
@@ -6595,16 +10512,16 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>479</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>488</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="15" t="s">
         <v>512</v>
       </c>
     </row>
@@ -6630,7 +10547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Tidying up the mess
</commit_message>
<xml_diff>
--- a/Documentation/Connections.xlsx
+++ b/Documentation/Connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="515">
   <si>
     <t>BEAM_TRIGGER_P&lt;0&gt;</t>
   </si>
@@ -5886,7 +5886,7 @@
   <dimension ref="A1:I302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6290,7 +6290,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>79</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>set_property PACKAGE_PIN T5 [get_ports {sysclk_40_i_p}]</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>80</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>set_property PACKAGE_PIN T4 [get_ports {sysclk_40_i_n}]</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>218</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>set_property PACKAGE_PIN E3 [get_ports {sysclk_50_o_p}]</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>set_property PACKAGE_PIN D3 [get_ports {sysclk_50_o_n}]</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -6407,7 +6407,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>113</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>set_property PACKAGE_PIN C2 [get_ports {i2c_reset}]</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>371</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>set_property PACKAGE_PIN F6 [get_ports {gpio}]</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>373</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>set_property PACKAGE_PIN C1 [get_ports {clk_gen_rst}]</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>375</v>
       </c>
@@ -6504,11 +6504,8 @@
       <c r="G25" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="11" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
@@ -6517,7 +6514,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>499</v>
       </c>
@@ -6534,7 +6531,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>500</v>
       </c>
@@ -6551,7 +6548,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>497</v>
       </c>
@@ -6569,7 +6566,7 @@
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>463</v>
       </c>
@@ -6586,7 +6583,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>462</v>
       </c>
@@ -6603,7 +6600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>458</v>
       </c>

</xml_diff>

<commit_message>
Added FPGA package pins to the lines related to the SFP connector
</commit_message>
<xml_diff>
--- a/Documentation/Connections.xlsx
+++ b/Documentation/Connections.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6AA01C-893C-4A26-8B83-DF978DE534CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMC" sheetId="1" r:id="rId1"/>
@@ -14,12 +15,12 @@
     <sheet name="Added SFP" sheetId="4" r:id="rId5"/>
     <sheet name="LEDs" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="527">
   <si>
     <t>BEAM_TRIGGER_P&lt;0&gt;</t>
   </si>
@@ -1566,12 +1567,48 @@
   </si>
   <si>
     <t>G27</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>N17</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>E1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1756,6 +1793,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1791,6 +1845,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1966,10 +2037,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I302"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -5882,11 +5953,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I302"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6399,219 +6470,221 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" ref="H22:H24" si="2">"set_property PACKAGE_PIN " &amp;E22 &amp; " [get_ports {" &amp; F22 &amp; "}]"</f>
+      <c r="H24" t="str">
+        <f t="shared" ref="H24:H26" si="2">"set_property PACKAGE_PIN " &amp;E24 &amp; " [get_ports {" &amp; F24 &amp; "}]"</f>
         <v>set_property PACKAGE_PIN C2 [get_ports {i2c_reset}]</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="H23" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="2"/>
         <v>set_property PACKAGE_PIN F6 [get_ports {gpio}]</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H24" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="2"/>
         <v>set_property PACKAGE_PIN C1 [get_ports {clk_gen_rst}]</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>486</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="14"/>
-    </row>
     <row r="27" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>499</v>
+        <v>375</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>502</v>
+        <v>444</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
       <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>242</v>
+      </c>
       <c r="F27" s="8"/>
       <c r="G27" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>504</v>
-      </c>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>497</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>513</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>514</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>463</v>
+        <v>500</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>462</v>
+        <v>497</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5" t="s">
-        <v>116</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>483</v>
+        <v>463</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>480</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="8" t="s">
+        <v>521</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="5" t="s">
         <v>116</v>
@@ -6619,16 +6692,18 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>482</v>
+        <v>462</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>481</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="8" t="s">
+        <v>522</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
         <v>116</v>
@@ -6636,1221 +6711,1247 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>505</v>
+        <v>458</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>510</v>
       </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="8" t="s">
+        <v>523</v>
+      </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>484</v>
+        <v>459</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="5"/>
+      <c r="A36" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>505</v>
+      </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="8" t="s">
+        <v>525</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H37" t="str">
-        <f t="shared" ref="H37:H50" si="3">"set_property PACKAGE_PIN " &amp;E37 &amp; " [get_ports {" &amp; F37 &amp; "}]"</f>
+      <c r="H39" t="str">
+        <f t="shared" ref="H39:H52" si="3">"set_property PACKAGE_PIN " &amp;E39 &amp; " [get_ports {" &amp; F39 &amp; "}]"</f>
         <v>set_property PACKAGE_PIN P5 [get_ports {cont_i[0]}]</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H38" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN P3 [get_ports {cont_i[1]}]</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H39" t="str">
+      <c r="H41" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN N6 [get_ports {cont_i[2]}]</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H40" t="str">
+      <c r="H42" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN L5 [get_ports {cont_i[3]}]</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H42" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN M1 [get_ports {spare_i[0]}]</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H43" t="str">
+      <c r="H45" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN N4 [get_ports {spare_i[1]}]</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G46" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H44" t="str">
+      <c r="H46" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN N1 [get_ports {spare_i[2]}]</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G47" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H45" t="str">
+      <c r="H47" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN M2 [get_ports {spare_i[3]}]</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G49" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H47" t="str">
+      <c r="H49" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN R5 [get_ports {triggers_i[0]}]</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G50" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H48" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN R2 [get_ports {triggers_i[1]}]</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G51" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H49" t="str">
+      <c r="H51" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN T1 [get_ports {triggers_i[2]}]</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="G52" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H50" t="str">
+      <c r="H52" t="str">
         <f t="shared" si="3"/>
         <v>set_property PACKAGE_PIN V1 [get_ports {triggers_i[3]}]</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G54" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H52" t="str">
-        <f t="shared" ref="H52:H60" si="4">"set_property PACKAGE_PIN " &amp;E52 &amp; " [get_ports {" &amp; F52 &amp; "}]"</f>
+      <c r="H54" t="str">
+        <f t="shared" ref="H54:H62" si="4">"set_property PACKAGE_PIN " &amp;E54 &amp; " [get_ports {" &amp; F54 &amp; "}]"</f>
         <v>set_property PACKAGE_PIN T6 [get_ports {busy_i[0]}]</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F55" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="G55" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H53" t="str">
+      <c r="H55" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN U3 [get_ports {busy_i[1]}]</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G56" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H54" t="str">
+      <c r="H56" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN T8 [get_ports {busy_i[2]}]</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="G57" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H55" t="str">
+      <c r="H57" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN L4 [get_ports {busy_i[3]}]</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F59" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="G59" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H57" t="str">
+      <c r="H59" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN L3 [get_ports {dut_clk_i[0]}]</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E60" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F60" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G60" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H58" t="str">
+      <c r="H60" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN F3 [get_ports {dut_clk_i[1]}]</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G61" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H59" t="str">
+      <c r="H61" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN D2 [get_ports {dut_clk_i[2]}]</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G62" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H60" t="str">
+      <c r="H62" t="str">
         <f t="shared" si="4"/>
         <v>set_property PACKAGE_PIN G3 [get_ports {dut_clk_i[3]}]</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F64" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G64" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H62" t="str">
-        <f t="shared" ref="H62:H75" si="5">"set_property PACKAGE_PIN " &amp;E62 &amp; " [get_ports {" &amp; F62 &amp; "}]"</f>
+      <c r="H64" t="str">
+        <f t="shared" ref="H64:H77" si="5">"set_property PACKAGE_PIN " &amp;E64 &amp; " [get_ports {" &amp; F64 &amp; "}]"</f>
         <v>set_property PACKAGE_PIN N5 [get_ports {cont_o[0]}]</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F65" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="G63" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H63" t="str">
+      <c r="H65" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN P4 [get_ports {cont_o[1]}]</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F66" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="G66" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H64" t="str">
+      <c r="H66" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN M6 [get_ports {cont_o[2]}]</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F67" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G67" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H65" t="str">
+      <c r="H67" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN L6 [get_ports {cont_o[3]}]</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E69" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F69" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G69" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H67" t="str">
+      <c r="H69" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN L1 [get_ports {spare_o[0]}]</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F70" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G70" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H68" t="str">
+      <c r="H70" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN M4 [get_ports {spare_o[1]}]</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F71" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G71" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H69" t="str">
+      <c r="H71" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN N2 [get_ports {spare_o[2]}]</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="G72" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H70" t="str">
+      <c r="H72" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN M3 [get_ports {spare_o[3]}]</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G74" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H72" t="str">
+      <c r="H74" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN R6 [get_ports {triggers_o[0]}]</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="G75" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H73" t="str">
+      <c r="H75" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN P2 [get_ports {triggers_o[1]}]</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E76" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="G76" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H74" t="str">
+      <c r="H76" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN R1 [get_ports {triggers_o[2]}]</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D77" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F77" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="G77" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H75" t="str">
+      <c r="H77" t="str">
         <f t="shared" si="5"/>
         <v>set_property PACKAGE_PIN U1 [get_ports {triggers_o[3]}]</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="5"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H77" t="str">
-        <f>"set_property PACKAGE_PIN " &amp;E77 &amp; " [get_ports {" &amp; F77 &amp; "}]"</f>
-        <v>set_property PACKAGE_PIN R7 [get_ports {busy_o[0]}]</v>
-      </c>
-    </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H78" t="str">
-        <f t="shared" ref="H78:H85" si="6">"set_property PACKAGE_PIN " &amp;E78 &amp; " [get_ports {" &amp; F78 &amp; "}]"</f>
-        <v>set_property PACKAGE_PIN U4 [get_ports {busy_o[1]}]</v>
-      </c>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H79" t="str">
+        <f>"set_property PACKAGE_PIN " &amp;E79 &amp; " [get_ports {" &amp; F79 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN R7 [get_ports {busy_o[0]}]</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" ref="H80:H87" si="6">"set_property PACKAGE_PIN " &amp;E80 &amp; " [get_ports {" &amp; F80 &amp; "}]"</f>
+        <v>set_property PACKAGE_PIN U4 [get_ports {busy_o[1]}]</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H81" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN R8 [get_ports {busy_o[2]}]</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D82" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E82" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="F82" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G82" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H80" t="str">
+      <c r="H82" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN K5 [get_ports {busy_o[3]}]</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="5"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D84" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="G82" s="5" t="s">
+      <c r="G84" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H82" t="str">
+      <c r="H84" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN K3 [get_ports {dut_clk_o[0]}]</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D85" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E85" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="F85" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G83" s="5" t="s">
+      <c r="G85" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H83" t="str">
+      <c r="H85" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN F4 [get_ports {dut_clk_o[1]}]</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D86" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E86" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="F86" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G84" s="5" t="s">
+      <c r="G86" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H84" t="str">
+      <c r="H86" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN E2 [get_ports {dut_clk_o[2]}]</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F87" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="G85" s="5" t="s">
+      <c r="G87" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H85" t="str">
+      <c r="H87" t="str">
         <f t="shared" si="6"/>
         <v>set_property PACKAGE_PIN G4 [get_ports {dut_clk_o[3]}]</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="5"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="5"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="5"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
@@ -7862,8 +7963,6 @@
       <c r="G88" s="5"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
       <c r="C89" s="5"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -9779,11 +9878,29 @@
       <c r="G301" s="5"/>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="4"/>
+      <c r="B302" s="4"/>
       <c r="C302" s="5"/>
       <c r="D302" s="4"/>
       <c r="E302" s="4"/>
       <c r="F302" s="4"/>
       <c r="G302" s="5"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="4"/>
+      <c r="B303" s="4"/>
+      <c r="C303" s="5"/>
+      <c r="D303" s="4"/>
+      <c r="E303" s="4"/>
+      <c r="F303" s="4"/>
+      <c r="G303" s="5"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C304" s="5"/>
+      <c r="D304" s="4"/>
+      <c r="E304" s="4"/>
+      <c r="F304" s="4"/>
+      <c r="G304" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9795,7 +9912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9959,7 +10076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10240,7 +10357,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10545,7 +10662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>